<commit_message>
create the endpoint for seeding
</commit_message>
<xml_diff>
--- a/docs/Data Set for Symptons Illnesses.xlsx
+++ b/docs/Data Set for Symptons Illnesses.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f084ede0c2fcfd21/Desktop/Software Development Exercise/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\source\repos\5COM1079-SDE-backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9131FB3B-BC32-4353-95B5-704ED65BF215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DCEAF9-11F7-4252-AF83-B8FC15B58168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Set" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -68,10 +57,6 @@
     <t>Asthma is a common lung condition that causes occasional breathing difficulties.</t>
   </si>
   <si>
-    <t xml:space="preserve">Breathlessness|Shortness of breath|Coughing|Tight chest|Wheezing|
-</t>
-  </si>
-  <si>
     <t>https://www.nhs.uk/conditions/asthma/</t>
   </si>
   <si>
@@ -427,13 +412,17 @@
   </si>
   <si>
     <t>https://www.nhs.uk/conditions/zika/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breathlessness|Shortness of breath|Coughing|Tight chest|Wheezing
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,10 +782,10 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" style="2" customWidth="1"/>
@@ -805,7 +794,7 @@
     <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -819,7 +808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="130.5">
+    <row r="2" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -833,7 +822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.5">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -841,416 +830,416 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="72.599999999999994">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="72.599999999999994">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="29.1">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="72.599999999999994">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.5">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="72.599999999999994">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="7" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="57.95">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="57.95">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="72.599999999999994">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="7" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="72.599999999999994">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="7" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="57.95">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="57.95">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="7" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="57.95">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="7" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="72.599999999999994">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="7" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="130.5">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="7" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="116.1">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="7" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="57.95">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="7" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="57.95">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="7" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="57.95">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="7" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="72.599999999999994">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="7" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="72.599999999999994">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="7" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="57.95">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="7" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="43.5">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="7" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="87">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="7" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="57.95">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="7" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="87">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="7" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="87">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="7" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="87">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="7" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="72.599999999999994">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>